<commit_message>
add filter using mysql detabase
</commit_message>
<xml_diff>
--- a/Backend/public/flightdetails/Book2.xlsx
+++ b/Backend/public/flightdetails/Book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACDBC5A-69B9-45F4-A801-C558D8F32E94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9E4BAE-68C5-406F-9163-D1A66D9BDC89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38BA9C54-E86A-4274-B85C-149D37B2029B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>SECTOR</t>
   </si>
@@ -69,15 +69,6 @@
     <t>SEATS_AVAILABLE</t>
   </si>
   <si>
-    <t>16-12-2022</t>
-  </si>
-  <si>
-    <t>17-12-2022</t>
-  </si>
-  <si>
-    <t>18-12-2022</t>
-  </si>
-  <si>
     <t>10:45:00</t>
   </si>
   <si>
@@ -85,6 +76,27 @@
   </si>
   <si>
     <t>02:45 MIN</t>
+  </si>
+  <si>
+    <t>LOGO</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>2022-12-17</t>
+  </si>
+  <si>
+    <t>2022-12-18</t>
+  </si>
+  <si>
+    <t>2022-12-19</t>
   </si>
 </sst>
 </file>
@@ -503,164 +515,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7EB925-2DE5-466F-8B51-DD401E6A0EAC}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.21875" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="28.44140625" customWidth="1"/>
-    <col min="9" max="9" width="26.6640625" customWidth="1"/>
-    <col min="10" max="10" width="29.33203125" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" customWidth="1"/>
+    <col min="11" max="11" width="29.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4">
         <v>14</v>
-      </c>
-      <c r="I2" s="4">
-        <v>7</v>
       </c>
       <c r="J2" s="4">
         <v>7</v>
       </c>
       <c r="K2" s="4">
+        <v>7</v>
+      </c>
+      <c r="L2" s="4">
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>14</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>9</v>
       </c>
-      <c r="J3" s="4">
+      <c r="K3" s="4">
         <v>5</v>
       </c>
-      <c r="K3" s="4">
+      <c r="L3" s="4">
         <v>9000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="4">
+      <c r="H4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="4">
         <v>14</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>4</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="4">
         <v>10</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <v>8000</v>
       </c>
     </row>

</xml_diff>